<commit_message>
Creation of html pages
</commit_message>
<xml_diff>
--- a/supplementary/S2_Table.xlsx
+++ b/supplementary/S2_Table.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maylis\Dropbox\Systematic review\Supplementary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maylis\Documents\cfss\RabiesScopingReview\supplementary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54165188-85B2-45BB-A83B-F4B02F4E8323}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D944E67-1B85-43AD-B56E-B3DE53D35C7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6108" yWindow="1272" windowWidth="17280" windowHeight="9060" xr2:uid="{77F8437B-3D34-4013-9B53-72D8A9C8486A}"/>
+    <workbookView xWindow="732" yWindow="1212" windowWidth="17280" windowHeight="5688" xr2:uid="{77F8437B-3D34-4013-9B53-72D8A9C8486A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="ST2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>

<commit_message>
URL to download supplementary materials
</commit_message>
<xml_diff>
--- a/supplementary/S2_Table.xlsx
+++ b/supplementary/S2_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maylis\Dropbox\Systematic review\Supplementary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD9C99A-9B95-4F32-842F-F863C4707191}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E803D471-49FA-4DB5-BF48-4417E38AE1BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="372" windowWidth="23256" windowHeight="12696" xr2:uid="{77F8437B-3D34-4013-9B53-72D8A9C8486A}"/>
   </bookViews>
@@ -393,7 +393,7 @@
     <t>Abbreviations: ACCTRAN, Accelerated Transformation; BSSVS, Bayesian Stochastic Search Variable Selection; DELTRAN, Delayed Transformation; DTA, Discrete Trait Analysis; GLM, Generalized Linear Model; tMRCA, time to the Most Recent Common Ancestor; WHO World Health Organization</t>
   </si>
   <si>
-    <t xml:space="preserve">S2 Table. Description of the phylogeographical models with an emphasis on data source and quality. </t>
+    <t xml:space="preserve">S2 Table. Description of the phylogeographical models with an emphasis on data source and potential sources of bias. </t>
   </si>
 </sst>
 </file>
@@ -1087,9 +1087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A5C2F6-915C-4C48-971B-E36655E383F8}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>